<commit_message>
feature: alien status note
</commit_message>
<xml_diff>
--- a/public/example/usage-import.xlsx
+++ b/public/example/usage-import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandytseng/Desktop/Project/taicol-物種學名管理工具/taicol/public/example/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taibif/Documents/00-GitHub/taicol-2021/public/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD97419C-D9FB-BD46-94A8-B074C3714631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601B672F-1EAA-A14C-BB9C-44EFDC8595C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40200" yWindow="5020" windowWidth="27460" windowHeight="15840" xr2:uid="{5E2458F6-5B21-7645-B9CB-A68269CDEE8D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{5E2458F6-5B21-7645-B9CB-A68269CDEE8D}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>rank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -95,6 +94,10 @@
   </si>
   <si>
     <t>common_name(language,area)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alien_status_note</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -171,7 +174,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24BD2BA-B27D-A54D-8E83-71A630B651AD}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -500,7 +503,7 @@
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="13">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="13">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -554,6 +557,9 @@
       </c>
       <c r="R1" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: new record, related name
</commit_message>
<xml_diff>
--- a/public/example/usage-import.xlsx
+++ b/public/example/usage-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taibif/Documents/00-GitHub/taicol-2021/public/example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601B672F-1EAA-A14C-BB9C-44EFDC8595C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB5CCA-22B3-4E47-931E-07520880B271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15760" xr2:uid="{5E2458F6-5B21-7645-B9CB-A68269CDEE8D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>rank</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -98,6 +98,10 @@
   </si>
   <si>
     <t>alien_status_note</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>is_new_record</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -489,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C24BD2BA-B27D-A54D-8E83-71A630B651AD}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="255" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="255" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -503,7 +507,7 @@
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="13">
+    <row r="1" spans="1:20" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -560,6 +564,9 @@
       </c>
       <c r="S1" s="2" t="s">
         <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>